<commit_message>
File changes and code writing for packaging data
</commit_message>
<xml_diff>
--- a/indexdata2018 review 10.9.18.xlsx
+++ b/indexdata2018 review 10.9.18.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbunn\Dropbox (Tax Foundation)\international-tax-competitiveness-index\2019 Index\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFC2F20-DB86-43D4-A821-532564046BA9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970B00FA-1377-4BA9-A4AD-6B65570D7D5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="150" windowWidth="29040" windowHeight="15840" tabRatio="962" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="962" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 minus 2017" sheetId="23" r:id="rId1"/>
@@ -926,7 +926,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="196">
   <si>
     <t>country</t>
   </si>
@@ -11734,7 +11734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45BBA53-8B08-40D6-A02B-E0D3FEBC5932}">
   <dimension ref="A1:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -63705,14 +63705,4623 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC2205A-E3D3-43FC-9CAE-2D3C369F6DC8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AP36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>0.3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="F2">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G2">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>37</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <v>0.1</v>
+      </c>
+      <c r="O2">
+        <v>50335.570469798658</v>
+      </c>
+      <c r="P2">
+        <v>0.49</v>
+      </c>
+      <c r="Q2">
+        <v>50</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1.2181395953081706</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0.245</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0.24280000000000002</v>
+      </c>
+      <c r="AC2">
+        <v>0.49</v>
+      </c>
+      <c r="AD2">
+        <v>2.1546129999999999</v>
+      </c>
+      <c r="AE2">
+        <v>1.3953283744731524</v>
+      </c>
+      <c r="AF2">
+        <v>4</v>
+      </c>
+      <c r="AG2">
+        <v>18</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>0.3</v>
+      </c>
+      <c r="AK2">
+        <v>0.1</v>
+      </c>
+      <c r="AL2">
+        <v>0.3</v>
+      </c>
+      <c r="AM2">
+        <v>45</v>
+      </c>
+      <c r="AN2">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>0.25</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>75</v>
+      </c>
+      <c r="E3">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="F3">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>46</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>0.2</v>
+      </c>
+      <c r="O3">
+        <v>37500</v>
+      </c>
+      <c r="P3">
+        <v>0.59</v>
+      </c>
+      <c r="Q3">
+        <v>35</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>0.13462119796448438</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="AC3">
+        <v>0.47964286</v>
+      </c>
+      <c r="AD3">
+        <v>7.8721480000000001</v>
+      </c>
+      <c r="AE3">
+        <v>1.136461890315154</v>
+      </c>
+      <c r="AF3">
+        <v>3</v>
+      </c>
+      <c r="AG3">
+        <v>50</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0.2</v>
+      </c>
+      <c r="AM3">
+        <v>91</v>
+      </c>
+      <c r="AN3">
+        <v>0.5</v>
+      </c>
+      <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>0.29580000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.622</v>
+      </c>
+      <c r="G4">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>21</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>0.21</v>
+      </c>
+      <c r="O4">
+        <v>31250</v>
+      </c>
+      <c r="P4">
+        <v>0.47</v>
+      </c>
+      <c r="Q4">
+        <v>75</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>0.70869963661052915</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>0.3</v>
+      </c>
+      <c r="AC4">
+        <v>0.60215737999999996</v>
+      </c>
+      <c r="AD4">
+        <v>1.0489010000000001</v>
+      </c>
+      <c r="AE4">
+        <v>1.2370516974072907</v>
+      </c>
+      <c r="AF4">
+        <v>2</v>
+      </c>
+      <c r="AG4">
+        <v>40</v>
+      </c>
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
+        <v>0.3</v>
+      </c>
+      <c r="AK4">
+        <v>0.3</v>
+      </c>
+      <c r="AL4">
+        <v>0.3</v>
+      </c>
+      <c r="AM4">
+        <v>95</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="F5">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>45</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>0.1242697</v>
+      </c>
+      <c r="O5">
+        <v>24000</v>
+      </c>
+      <c r="P5">
+        <v>0.49</v>
+      </c>
+      <c r="Q5">
+        <v>50</v>
+      </c>
+      <c r="R5">
+        <v>0.5</v>
+      </c>
+      <c r="S5">
+        <v>2.054426247046357</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0.26750000000000002</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0.39343524000000002</v>
+      </c>
+      <c r="AC5">
+        <v>0.53529599999999999</v>
+      </c>
+      <c r="AD5">
+        <v>4.2600660000000001</v>
+      </c>
+      <c r="AE5">
+        <v>1.184405373849633</v>
+      </c>
+      <c r="AF5">
+        <v>3</v>
+      </c>
+      <c r="AG5">
+        <v>36</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>0.5</v>
+      </c>
+      <c r="AJ5">
+        <v>0.25</v>
+      </c>
+      <c r="AK5">
+        <v>0.25</v>
+      </c>
+      <c r="AL5">
+        <v>0.25</v>
+      </c>
+      <c r="AM5">
+        <v>96</v>
+      </c>
+      <c r="AN5">
+        <v>0.33333333300000001</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>0.25</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>42</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>0.19</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0.63</v>
+      </c>
+      <c r="Q6">
+        <v>124</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0.60520837213797329</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0.35</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0.13333333</v>
+      </c>
+      <c r="AC6">
+        <v>0.35</v>
+      </c>
+      <c r="AD6">
+        <v>7.7260530000000003</v>
+      </c>
+      <c r="AE6">
+        <v>1.137130991775757</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>125</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0.35</v>
+      </c>
+      <c r="AK6">
+        <v>0.35</v>
+      </c>
+      <c r="AL6">
+        <v>0.3</v>
+      </c>
+      <c r="AM6">
+        <v>32</v>
+      </c>
+      <c r="AN6">
+        <v>0.5</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>0.19</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>0.874</v>
+      </c>
+      <c r="F7">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="G7">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>53</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>0.21</v>
+      </c>
+      <c r="O7">
+        <v>76923.076923076922</v>
+      </c>
+      <c r="P7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Q7">
+        <v>108</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0.15582555724473959</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0.15</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>0.15</v>
+      </c>
+      <c r="AC7">
+        <v>0.311</v>
+      </c>
+      <c r="AD7">
+        <v>0.34797400000000001</v>
+      </c>
+      <c r="AE7">
+        <v>1.1169971676870944</v>
+      </c>
+      <c r="AF7">
+        <v>2</v>
+      </c>
+      <c r="AG7">
+        <v>87</v>
+      </c>
+      <c r="AH7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
+        <v>0.15</v>
+      </c>
+      <c r="AK7">
+        <v>0.15</v>
+      </c>
+      <c r="AL7">
+        <v>0.15</v>
+      </c>
+      <c r="AM7">
+        <v>87</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AP7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>0.22</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>60</v>
+      </c>
+      <c r="E8">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="F8">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G8">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>25</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>0.25</v>
+      </c>
+      <c r="O8">
+        <v>6793.478260869565</v>
+      </c>
+      <c r="P8">
+        <v>0.59</v>
+      </c>
+      <c r="Q8">
+        <v>40</v>
+      </c>
+      <c r="R8">
+        <v>0.5</v>
+      </c>
+      <c r="S8">
+        <v>0.86008887974339188</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0.42</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0.42</v>
+      </c>
+      <c r="AC8">
+        <v>0.55793999999999999</v>
+      </c>
+      <c r="AD8">
+        <v>1.2607029999999999</v>
+      </c>
+      <c r="AE8">
+        <v>1.2726913010902041</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>65</v>
+      </c>
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>0.27</v>
+      </c>
+      <c r="AK8">
+        <v>0.22</v>
+      </c>
+      <c r="AL8">
+        <v>0.22</v>
+      </c>
+      <c r="AM8">
+        <v>74</v>
+      </c>
+      <c r="AN8">
+        <v>0.83333333300000001</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+      <c r="AP8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <v>0.2</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>0.2</v>
+      </c>
+      <c r="O9">
+        <v>74074.074074074073</v>
+      </c>
+      <c r="P9">
+        <v>0.7</v>
+      </c>
+      <c r="Q9">
+        <v>14</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0.20053939386678538</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0.2</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0.21280000000000002</v>
+      </c>
+      <c r="AD9">
+        <v>0.14828</v>
+      </c>
+      <c r="AE9">
+        <v>1.0539919995277536</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>31</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <v>1</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0.1</v>
+      </c>
+      <c r="AM9">
+        <v>57</v>
+      </c>
+      <c r="AN9">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO9">
+        <v>1</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10">
+        <v>0.2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="F10">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="G10">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>21</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>0.24</v>
+      </c>
+      <c r="O10">
+        <v>10989.010989010989</v>
+      </c>
+      <c r="P10">
+        <v>0.54</v>
+      </c>
+      <c r="Q10">
+        <v>24</v>
+      </c>
+      <c r="R10">
+        <v>0.5</v>
+      </c>
+      <c r="S10">
+        <v>0.45917407182519443</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>0.34</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="AC10">
+        <v>0.58349397000000003</v>
+      </c>
+      <c r="AD10">
+        <v>1.8517250000000001</v>
+      </c>
+      <c r="AE10">
+        <v>1.3036626509615676</v>
+      </c>
+      <c r="AF10">
+        <v>3</v>
+      </c>
+      <c r="AG10">
+        <v>48</v>
+      </c>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <v>0.2</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0.2</v>
+      </c>
+      <c r="AM10">
+        <v>86</v>
+      </c>
+      <c r="AN10">
+        <v>0.83333333300000001</v>
+      </c>
+      <c r="AO10">
+        <v>1</v>
+      </c>
+      <c r="AP10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>0.34429999999999999</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="F11">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="G11">
+        <v>0.87</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>28</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>0.2</v>
+      </c>
+      <c r="O11">
+        <v>101481.48148148147</v>
+      </c>
+      <c r="P11">
+        <v>0.48</v>
+      </c>
+      <c r="Q11">
+        <v>31</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1.7012127024606762</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>0.34429999999999999</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0.34</v>
+      </c>
+      <c r="AC11">
+        <v>0.550875</v>
+      </c>
+      <c r="AD11">
+        <v>14.576138</v>
+      </c>
+      <c r="AE11">
+        <v>1.270283551051838</v>
+      </c>
+      <c r="AF11">
+        <v>2</v>
+      </c>
+      <c r="AG11">
+        <v>80</v>
+      </c>
+      <c r="AH11">
+        <v>0.95</v>
+      </c>
+      <c r="AI11">
+        <v>0.88</v>
+      </c>
+      <c r="AJ11">
+        <v>0.3</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="AM11">
+        <v>107</v>
+      </c>
+      <c r="AN11">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO11">
+        <v>1</v>
+      </c>
+      <c r="AP11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>0.29825000000000002</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>60</v>
+      </c>
+      <c r="E12">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G12">
+        <v>0.87</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>41</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>6</v>
+      </c>
+      <c r="N12">
+        <v>0.19</v>
+      </c>
+      <c r="O12">
+        <v>22435.897435897434</v>
+      </c>
+      <c r="P12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Q12">
+        <v>43</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0.31606464248403543</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0.26374999999999998</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0.26374999999999998</v>
+      </c>
+      <c r="AC12">
+        <v>0.47475000000000001</v>
+      </c>
+      <c r="AD12">
+        <v>5.4032249999999999</v>
+      </c>
+      <c r="AE12">
+        <v>1.1042040013986685</v>
+      </c>
+      <c r="AF12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>134</v>
+      </c>
+      <c r="AH12">
+        <v>0.95</v>
+      </c>
+      <c r="AI12">
+        <v>0.95</v>
+      </c>
+      <c r="AJ12">
+        <v>0.25</v>
+      </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>0.15</v>
+      </c>
+      <c r="AM12">
+        <v>96</v>
+      </c>
+      <c r="AN12">
+        <v>0.5</v>
+      </c>
+      <c r="AO12">
+        <v>0</v>
+      </c>
+      <c r="AP12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="F13">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G13">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>78</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>6</v>
+      </c>
+      <c r="N13">
+        <v>0.24</v>
+      </c>
+      <c r="O13">
+        <v>16666.666666666668</v>
+      </c>
+      <c r="P13">
+        <v>0.37</v>
+      </c>
+      <c r="Q13">
+        <v>69</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1.5008500258376438</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0.15</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0.15</v>
+      </c>
+      <c r="AC13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AD13">
+        <v>3.9284680000000001</v>
+      </c>
+      <c r="AE13">
+        <v>1.2488759720212623</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AG13">
+        <v>46</v>
+      </c>
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0.15</v>
+      </c>
+      <c r="AK13">
+        <v>0.15</v>
+      </c>
+      <c r="AL13">
+        <v>0.2</v>
+      </c>
+      <c r="AM13">
+        <v>57</v>
+      </c>
+      <c r="AN13">
+        <v>0.5</v>
+      </c>
+      <c r="AO13">
+        <v>1</v>
+      </c>
+      <c r="AP13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14">
+        <v>0.09</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2.5</v>
+      </c>
+      <c r="E14">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="F14">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G14">
+        <v>0.87</v>
+      </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>35</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>7</v>
+      </c>
+      <c r="N14">
+        <v>0.27</v>
+      </c>
+      <c r="O14">
+        <v>59259.259259259263</v>
+      </c>
+      <c r="P14">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q14">
+        <v>96</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>0.50685386329674798</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>0.15</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0.15</v>
+      </c>
+      <c r="AC14">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>1</v>
+      </c>
+      <c r="AF14">
+        <v>2</v>
+      </c>
+      <c r="AG14">
+        <v>146</v>
+      </c>
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AI14">
+        <v>1</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>80</v>
+      </c>
+      <c r="AN14">
+        <v>0.33333333300000001</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15">
+        <v>0.2</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>0.86</v>
+      </c>
+      <c r="F15">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="G15">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="H15">
+        <v>0.5</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>40</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>7</v>
+      </c>
+      <c r="N15">
+        <v>0.24</v>
+      </c>
+      <c r="O15">
+        <v>6944.4444444444443</v>
+      </c>
+      <c r="P15">
+        <v>0.46</v>
+      </c>
+      <c r="Q15">
+        <v>40</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1.475661032120082</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0.2</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0.22</v>
+      </c>
+      <c r="AC15">
+        <v>0.44390400000000002</v>
+      </c>
+      <c r="AD15">
+        <v>1.171853</v>
+      </c>
+      <c r="AE15">
+        <v>1.2751459233613365</v>
+      </c>
+      <c r="AF15">
+        <v>13</v>
+      </c>
+      <c r="AG15">
+        <v>60</v>
+      </c>
+      <c r="AH15">
+        <v>1</v>
+      </c>
+      <c r="AI15">
+        <v>1</v>
+      </c>
+      <c r="AJ15">
+        <v>0.2</v>
+      </c>
+      <c r="AK15">
+        <v>0.12</v>
+      </c>
+      <c r="AL15">
+        <v>0.2</v>
+      </c>
+      <c r="AM15">
+        <v>43</v>
+      </c>
+      <c r="AN15">
+        <v>0.83333333300000001</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16">
+        <v>0.125</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="F16">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G16">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="H16">
+        <v>0.5</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>12</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>7</v>
+      </c>
+      <c r="N16">
+        <v>0.23</v>
+      </c>
+      <c r="O16">
+        <v>92592.592592592584</v>
+      </c>
+      <c r="P16">
+        <v>0.49</v>
+      </c>
+      <c r="Q16">
+        <v>30</v>
+      </c>
+      <c r="R16">
+        <v>0.5</v>
+      </c>
+      <c r="S16">
+        <v>0.4622340710852299</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>0.33</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0.51</v>
+      </c>
+      <c r="AC16">
+        <v>0.52</v>
+      </c>
+      <c r="AD16">
+        <v>1.9293670000000001</v>
+      </c>
+      <c r="AE16">
+        <v>1.6765606236686132</v>
+      </c>
+      <c r="AF16">
+        <v>1</v>
+      </c>
+      <c r="AG16">
+        <v>40</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>1</v>
+      </c>
+      <c r="AJ16">
+        <v>0.2</v>
+      </c>
+      <c r="AK16">
+        <v>0.2</v>
+      </c>
+      <c r="AL16">
+        <v>0.2</v>
+      </c>
+      <c r="AM16">
+        <v>73</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>1</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17">
+        <v>0.23</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>0.87</v>
+      </c>
+      <c r="F17">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="G17">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>110</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>19</v>
+      </c>
+      <c r="N17">
+        <v>0.17</v>
+      </c>
+      <c r="O17">
+        <v>25850.13054830287</v>
+      </c>
+      <c r="P17">
+        <v>0.63</v>
+      </c>
+      <c r="Q17">
+        <v>65</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1.8148649891001376</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0.25</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>0.33</v>
+      </c>
+      <c r="AC17">
+        <v>0.5</v>
+      </c>
+      <c r="AD17">
+        <v>4.3248100000000003</v>
+      </c>
+      <c r="AE17">
+        <v>1.7700548894450712</v>
+      </c>
+      <c r="AF17">
+        <v>12</v>
+      </c>
+      <c r="AG17">
+        <v>60</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
+        <v>0.3</v>
+      </c>
+      <c r="AK17">
+        <v>0.23</v>
+      </c>
+      <c r="AL17">
+        <v>0.23</v>
+      </c>
+      <c r="AM17">
+        <v>55</v>
+      </c>
+      <c r="AN17">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18">
+        <v>0.27806399999999998</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>80</v>
+      </c>
+      <c r="E18">
+        <v>0.76</v>
+      </c>
+      <c r="F18">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="G18">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>39</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>11</v>
+      </c>
+      <c r="N18">
+        <v>0.22</v>
+      </c>
+      <c r="O18">
+        <v>41666.666666666672</v>
+      </c>
+      <c r="P18">
+        <v>0.37</v>
+      </c>
+      <c r="Q18">
+        <v>30</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>0.71022043561406334</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>0.26</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0.26</v>
+      </c>
+      <c r="AC18">
+        <v>0.52765572999999999</v>
+      </c>
+      <c r="AD18">
+        <v>2.7003689999999998</v>
+      </c>
+      <c r="AE18">
+        <v>1.2173212511757805</v>
+      </c>
+      <c r="AF18">
+        <v>1</v>
+      </c>
+      <c r="AG18">
+        <v>169</v>
+      </c>
+      <c r="AH18">
+        <v>0.95</v>
+      </c>
+      <c r="AI18">
+        <v>0.95</v>
+      </c>
+      <c r="AJ18">
+        <v>0.26</v>
+      </c>
+      <c r="AK18">
+        <v>0.26</v>
+      </c>
+      <c r="AL18">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AM18">
+        <v>102</v>
+      </c>
+      <c r="AN18">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO18">
+        <v>1</v>
+      </c>
+      <c r="AP18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19">
+        <v>0.2974</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>0.77</v>
+      </c>
+      <c r="F19">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G19">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>38</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>9</v>
+      </c>
+      <c r="N19">
+        <v>0.08</v>
+      </c>
+      <c r="O19">
+        <v>100000</v>
+      </c>
+      <c r="P19">
+        <v>0.7</v>
+      </c>
+      <c r="Q19">
+        <v>21</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1.3706552039042341</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0.20315</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0.20319999999999999</v>
+      </c>
+      <c r="AC19">
+        <v>0.56077164999999995</v>
+      </c>
+      <c r="AD19">
+        <v>8.5024390000000007</v>
+      </c>
+      <c r="AE19">
+        <v>1.1342220524429814</v>
+      </c>
+      <c r="AF19">
+        <v>2</v>
+      </c>
+      <c r="AG19">
+        <v>92</v>
+      </c>
+      <c r="AH19">
+        <v>0.95</v>
+      </c>
+      <c r="AI19">
+        <v>0</v>
+      </c>
+      <c r="AJ19">
+        <v>0.2</v>
+      </c>
+      <c r="AK19">
+        <v>0.2</v>
+      </c>
+      <c r="AL19">
+        <v>0.2</v>
+      </c>
+      <c r="AM19">
+        <v>70</v>
+      </c>
+      <c r="AN19">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO19">
+        <v>0</v>
+      </c>
+      <c r="AP19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>7.5</v>
+      </c>
+      <c r="E20">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="F20">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="G20">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>48</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>0.1</v>
+      </c>
+      <c r="O20">
+        <v>27428.571428571428</v>
+      </c>
+      <c r="P20">
+        <v>0.69</v>
+      </c>
+      <c r="Q20">
+        <v>48</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>0.2393750070208199</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>0.40279999999999999</v>
+      </c>
+      <c r="AC20">
+        <v>0.43239865999999999</v>
+      </c>
+      <c r="AD20">
+        <v>3.8392599999999999</v>
+      </c>
+      <c r="AE20">
+        <v>1.2678292317482871</v>
+      </c>
+      <c r="AF20">
+        <v>2</v>
+      </c>
+      <c r="AG20">
+        <v>72</v>
+      </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <v>0</v>
+      </c>
+      <c r="AJ20">
+        <v>0.2</v>
+      </c>
+      <c r="AK20">
+        <v>0.2</v>
+      </c>
+      <c r="AL20">
+        <v>0.2</v>
+      </c>
+      <c r="AM20">
+        <v>93</v>
+      </c>
+      <c r="AN20">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
+      <c r="AP20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21">
+        <v>0.2</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>100</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>23</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>0.21</v>
+      </c>
+      <c r="O21">
+        <v>80000</v>
+      </c>
+      <c r="P21">
+        <v>0.51</v>
+      </c>
+      <c r="Q21">
+        <v>66</v>
+      </c>
+      <c r="R21">
+        <v>0.5</v>
+      </c>
+      <c r="S21">
+        <v>0.52702026606513852</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0.2</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0.21425</v>
+      </c>
+      <c r="AD21">
+        <v>7.3729000000000003E-2</v>
+      </c>
+      <c r="AE21">
+        <v>1.040034121053969</v>
+      </c>
+      <c r="AF21">
+        <v>1</v>
+      </c>
+      <c r="AG21">
+        <v>80</v>
+      </c>
+      <c r="AH21">
+        <v>1</v>
+      </c>
+      <c r="AI21">
+        <v>1</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>0</v>
+      </c>
+      <c r="AM21">
+        <v>61</v>
+      </c>
+      <c r="AN21">
+        <v>0</v>
+      </c>
+      <c r="AO21">
+        <v>1</v>
+      </c>
+      <c r="AP21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22">
+        <v>0.2601</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <v>0.871</v>
+      </c>
+      <c r="F22">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G22">
+        <v>0.87</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>19</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+      <c r="M22">
+        <v>6</v>
+      </c>
+      <c r="N22">
+        <v>0.17</v>
+      </c>
+      <c r="O22">
+        <v>33333.333333333336</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>22</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>5.4022869393458947E-2</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
+        <v>0.21</v>
+      </c>
+      <c r="AC22">
+        <v>0.42820000000000003</v>
+      </c>
+      <c r="AD22">
+        <v>2.8058000000000001</v>
+      </c>
+      <c r="AE22">
+        <v>1.3995411900495283</v>
+      </c>
+      <c r="AF22">
+        <v>12</v>
+      </c>
+      <c r="AG22">
+        <v>14</v>
+      </c>
+      <c r="AH22">
+        <v>1</v>
+      </c>
+      <c r="AI22">
+        <v>1</v>
+      </c>
+      <c r="AJ22">
+        <v>0.15</v>
+      </c>
+      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>0</v>
+      </c>
+      <c r="AM22">
+        <v>81</v>
+      </c>
+      <c r="AN22">
+        <v>0</v>
+      </c>
+      <c r="AO22">
+        <v>0</v>
+      </c>
+      <c r="AP22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23">
+        <v>0.3</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="F23">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="G23">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>102</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>0.16</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0.32</v>
+      </c>
+      <c r="Q23">
+        <v>100</v>
+      </c>
+      <c r="R23">
+        <v>0.5</v>
+      </c>
+      <c r="S23">
+        <v>0.18821571499745496</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0.1</v>
+      </c>
+      <c r="AA23">
+        <v>1</v>
+      </c>
+      <c r="AB23">
+        <v>0.17142857</v>
+      </c>
+      <c r="AC23">
+        <v>0.35</v>
+      </c>
+      <c r="AD23">
+        <v>25.40869</v>
+      </c>
+      <c r="AE23">
+        <v>1.2007927060434405</v>
+      </c>
+      <c r="AF23">
+        <v>2</v>
+      </c>
+      <c r="AG23">
+        <v>39</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0.1</v>
+      </c>
+      <c r="AK23">
+        <v>0.35</v>
+      </c>
+      <c r="AL23">
+        <v>0.35</v>
+      </c>
+      <c r="AM23">
+        <v>58</v>
+      </c>
+      <c r="AN23">
+        <v>1</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24">
+        <v>0.25</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="F24">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="G24">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>21</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>7</v>
+      </c>
+      <c r="N24">
+        <v>0.21</v>
+      </c>
+      <c r="O24">
+        <v>1640.2439024390244</v>
+      </c>
+      <c r="P24">
+        <v>0.48</v>
+      </c>
+      <c r="Q24">
+        <v>34</v>
+      </c>
+      <c r="R24">
+        <v>0.5</v>
+      </c>
+      <c r="S24">
+        <v>0.67266015732664974</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>1</v>
+      </c>
+      <c r="AB24">
+        <v>0.25</v>
+      </c>
+      <c r="AC24">
+        <v>0.52269551999999997</v>
+      </c>
+      <c r="AD24">
+        <v>1.385089</v>
+      </c>
+      <c r="AE24">
+        <v>1.3671686126021072</v>
+      </c>
+      <c r="AF24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>64</v>
+      </c>
+      <c r="AH24">
+        <v>1</v>
+      </c>
+      <c r="AI24">
+        <v>1</v>
+      </c>
+      <c r="AJ24">
+        <v>0.15</v>
+      </c>
+      <c r="AK24">
+        <v>0</v>
+      </c>
+      <c r="AL24">
+        <v>0</v>
+      </c>
+      <c r="AM24">
+        <v>97</v>
+      </c>
+      <c r="AN24">
+        <v>0</v>
+      </c>
+      <c r="AO24">
+        <v>1</v>
+      </c>
+      <c r="AP24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>100</v>
+      </c>
+      <c r="E25">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="F25">
+        <v>0.307</v>
+      </c>
+      <c r="G25">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H25">
+        <v>0.5</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>34</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>4</v>
+      </c>
+      <c r="N25">
+        <v>0.15</v>
+      </c>
+      <c r="O25">
+        <v>40816.326530612248</v>
+      </c>
+      <c r="P25">
+        <v>0.97</v>
+      </c>
+      <c r="Q25">
+        <v>47</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>2.1116201452969072</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>1</v>
+      </c>
+      <c r="AB25">
+        <v>6.9444439999999996E-2</v>
+      </c>
+      <c r="AC25">
+        <v>0.33</v>
+      </c>
+      <c r="AD25">
+        <v>1.19</v>
+      </c>
+      <c r="AE25">
+        <v>1.4659545392745716</v>
+      </c>
+      <c r="AF25">
+        <v>2</v>
+      </c>
+      <c r="AG25">
+        <v>59</v>
+      </c>
+      <c r="AH25">
+        <v>1</v>
+      </c>
+      <c r="AI25">
+        <v>1</v>
+      </c>
+      <c r="AJ25">
+        <v>0.3</v>
+      </c>
+      <c r="AK25">
+        <v>0.15</v>
+      </c>
+      <c r="AL25">
+        <v>0.15</v>
+      </c>
+      <c r="AM25">
+        <v>40</v>
+      </c>
+      <c r="AN25">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO25">
+        <v>0</v>
+      </c>
+      <c r="AP25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26">
+        <v>0.23</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>100</v>
+      </c>
+      <c r="E26">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="F26">
+        <v>0.374</v>
+      </c>
+      <c r="G26">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>24</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+      <c r="N26">
+        <v>0.25</v>
+      </c>
+      <c r="O26">
+        <v>4950.4950495049507</v>
+      </c>
+      <c r="P26">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="Q26">
+        <v>44</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>0.26294741365233104</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0.23</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <v>0.30590000000000001</v>
+      </c>
+      <c r="AC26">
+        <v>0.4672</v>
+      </c>
+      <c r="AD26">
+        <v>1.616943</v>
+      </c>
+      <c r="AE26">
+        <v>1.2482480581223094</v>
+      </c>
+      <c r="AF26">
+        <v>1</v>
+      </c>
+      <c r="AG26">
+        <v>15</v>
+      </c>
+      <c r="AH26">
+        <v>0.97</v>
+      </c>
+      <c r="AI26">
+        <v>1</v>
+      </c>
+      <c r="AJ26">
+        <v>0.25</v>
+      </c>
+      <c r="AK26">
+        <v>0</v>
+      </c>
+      <c r="AL26">
+        <v>0</v>
+      </c>
+      <c r="AM26">
+        <v>88</v>
+      </c>
+      <c r="AN26">
+        <v>0.83333333300000001</v>
+      </c>
+      <c r="AO26">
+        <v>1</v>
+      </c>
+      <c r="AP26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27">
+        <v>0.19</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>2.5</v>
+      </c>
+      <c r="E27">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="F27">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="G27">
+        <v>0.87</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>59</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <v>0.23</v>
+      </c>
+      <c r="O27">
+        <v>111731.84357541898</v>
+      </c>
+      <c r="P27">
+        <v>0.44</v>
+      </c>
+      <c r="Q27">
+        <v>98</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>1.6133174818625202</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27">
+        <v>1</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>0.19</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0.19</v>
+      </c>
+      <c r="AC27">
+        <v>0.39908084999999999</v>
+      </c>
+      <c r="AD27">
+        <v>2.0307599999999999</v>
+      </c>
+      <c r="AE27">
+        <v>1.0373301700844437</v>
+      </c>
+      <c r="AF27">
+        <v>2</v>
+      </c>
+      <c r="AG27">
+        <v>103</v>
+      </c>
+      <c r="AH27">
+        <v>1</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0.19</v>
+      </c>
+      <c r="AK27">
+        <v>0.2</v>
+      </c>
+      <c r="AL27">
+        <v>0.2</v>
+      </c>
+      <c r="AM27">
+        <v>82</v>
+      </c>
+      <c r="AN27">
+        <v>0.83333333300000001</v>
+      </c>
+      <c r="AO27">
+        <v>1</v>
+      </c>
+      <c r="AP27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28">
+        <v>0.315</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>3.5</v>
+      </c>
+      <c r="E28">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="F28">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="G28">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H28">
+        <v>0.5</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>63</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>6</v>
+      </c>
+      <c r="N28">
+        <v>0.23</v>
+      </c>
+      <c r="O28">
+        <v>16949.152542372882</v>
+      </c>
+      <c r="P28">
+        <v>0.48</v>
+      </c>
+      <c r="Q28">
+        <v>90</v>
+      </c>
+      <c r="R28">
+        <v>0.5</v>
+      </c>
+      <c r="S28">
+        <v>0.50819985062170658</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="Z28">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AB28">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AC28">
+        <v>0.61026899999999995</v>
+      </c>
+      <c r="AD28">
+        <v>15.611608</v>
+      </c>
+      <c r="AE28">
+        <v>1.2632683636545734</v>
+      </c>
+      <c r="AF28">
+        <v>1</v>
+      </c>
+      <c r="AG28">
+        <v>90</v>
+      </c>
+      <c r="AH28">
+        <v>1</v>
+      </c>
+      <c r="AI28">
+        <v>1</v>
+      </c>
+      <c r="AJ28">
+        <v>0.25</v>
+      </c>
+      <c r="AK28">
+        <v>0.25</v>
+      </c>
+      <c r="AL28">
+        <v>0.25</v>
+      </c>
+      <c r="AM28">
+        <v>79</v>
+      </c>
+      <c r="AN28">
+        <v>0.83333333300000001</v>
+      </c>
+      <c r="AO28">
+        <v>1</v>
+      </c>
+      <c r="AP28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29">
+        <v>0.21</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>0.874</v>
+      </c>
+      <c r="F29">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="G29">
+        <v>0.87</v>
+      </c>
+      <c r="H29">
+        <v>0.5</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>46</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>6</v>
+      </c>
+      <c r="N29">
+        <v>0.2</v>
+      </c>
+      <c r="O29">
+        <v>101612.24489795919</v>
+      </c>
+      <c r="P29">
+        <v>0.48</v>
+      </c>
+      <c r="Q29">
+        <v>84</v>
+      </c>
+      <c r="R29">
+        <v>0.5</v>
+      </c>
+      <c r="S29">
+        <v>0.37563601672976898</v>
+      </c>
+      <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>0</v>
+      </c>
+      <c r="Y29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <v>0.21</v>
+      </c>
+      <c r="AA29">
+        <v>0</v>
+      </c>
+      <c r="AB29">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AC29">
+        <v>0.35049999999999998</v>
+      </c>
+      <c r="AD29">
+        <v>3.5395620000000001</v>
+      </c>
+      <c r="AE29">
+        <v>1.1127861207957699</v>
+      </c>
+      <c r="AF29">
+        <v>1</v>
+      </c>
+      <c r="AG29">
+        <v>62</v>
+      </c>
+      <c r="AH29">
+        <v>1</v>
+      </c>
+      <c r="AI29">
+        <v>0</v>
+      </c>
+      <c r="AJ29">
+        <v>0.35</v>
+      </c>
+      <c r="AK29">
+        <v>0.19</v>
+      </c>
+      <c r="AL29">
+        <v>0.19</v>
+      </c>
+      <c r="AM29">
+        <v>67</v>
+      </c>
+      <c r="AN29">
+        <v>0</v>
+      </c>
+      <c r="AO29">
+        <v>1</v>
+      </c>
+      <c r="AP29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30">
+        <v>0.19</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>50</v>
+      </c>
+      <c r="E30">
+        <v>0.87</v>
+      </c>
+      <c r="F30">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G30">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="H30">
+        <v>0.5</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>86</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>8</v>
+      </c>
+      <c r="N30">
+        <v>0.22</v>
+      </c>
+      <c r="O30">
+        <v>83333.333333333343</v>
+      </c>
+      <c r="P30">
+        <v>0.6</v>
+      </c>
+      <c r="Q30">
+        <v>69</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>0.36217667300492123</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="V30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <v>1</v>
+      </c>
+      <c r="AB30">
+        <v>0.25</v>
+      </c>
+      <c r="AC30">
+        <v>0.61049999999999993</v>
+      </c>
+      <c r="AD30">
+        <v>5.0394180000000004</v>
+      </c>
+      <c r="AE30">
+        <v>1.1538371326530812</v>
+      </c>
+      <c r="AF30">
+        <v>1</v>
+      </c>
+      <c r="AG30">
+        <v>90</v>
+      </c>
+      <c r="AH30">
+        <v>0.95</v>
+      </c>
+      <c r="AI30">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AJ30">
+        <v>0.15</v>
+      </c>
+      <c r="AK30">
+        <v>0.15</v>
+      </c>
+      <c r="AL30">
+        <v>0.15</v>
+      </c>
+      <c r="AM30">
+        <v>58</v>
+      </c>
+      <c r="AN30">
+        <v>0</v>
+      </c>
+      <c r="AO30">
+        <v>1</v>
+      </c>
+      <c r="AP30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31">
+        <v>0.25</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+      <c r="E31">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="F31">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G31">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="H31">
+        <v>0.5</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>33</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>7</v>
+      </c>
+      <c r="N31">
+        <v>0.21</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0.41</v>
+      </c>
+      <c r="Q31">
+        <v>35</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>0.62946857646953369</v>
+      </c>
+      <c r="T31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <v>1</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>1</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>0.23</v>
+      </c>
+      <c r="AA31">
+        <v>0</v>
+      </c>
+      <c r="AB31">
+        <v>0.23</v>
+      </c>
+      <c r="AC31">
+        <v>0.435</v>
+      </c>
+      <c r="AD31">
+        <v>2.4443090000000001</v>
+      </c>
+      <c r="AE31">
+        <v>1.2204405943878098</v>
+      </c>
+      <c r="AF31">
+        <v>1</v>
+      </c>
+      <c r="AG31">
+        <v>84</v>
+      </c>
+      <c r="AH31">
+        <v>1</v>
+      </c>
+      <c r="AI31">
+        <v>1</v>
+      </c>
+      <c r="AJ31">
+        <v>0.19</v>
+      </c>
+      <c r="AK31">
+        <v>0.19</v>
+      </c>
+      <c r="AL31">
+        <v>0.24</v>
+      </c>
+      <c r="AM31">
+        <v>89</v>
+      </c>
+      <c r="AN31">
+        <v>0.5</v>
+      </c>
+      <c r="AO31">
+        <v>1</v>
+      </c>
+      <c r="AP31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32">
+        <v>0.22</v>
+      </c>
+      <c r="C32">
+        <v>1.5</v>
+      </c>
+      <c r="D32">
+        <v>100</v>
+      </c>
+      <c r="E32">
+        <v>0.86</v>
+      </c>
+      <c r="F32">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G32">
+        <v>0.86</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>50</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>4</v>
+      </c>
+      <c r="N32">
+        <v>0.25</v>
+      </c>
+      <c r="O32">
+        <v>3303.964757709251</v>
+      </c>
+      <c r="P32">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q32">
+        <v>36</v>
+      </c>
+      <c r="R32">
+        <v>0.5</v>
+      </c>
+      <c r="S32">
+        <v>0.55064162160494157</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>1</v>
+      </c>
+      <c r="Z32">
+        <v>0.3</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <v>0.3</v>
+      </c>
+      <c r="AC32">
+        <v>0.60119999999999996</v>
+      </c>
+      <c r="AD32">
+        <v>1.49848</v>
+      </c>
+      <c r="AE32">
+        <v>1.231902977263251</v>
+      </c>
+      <c r="AF32">
+        <v>1</v>
+      </c>
+      <c r="AG32">
+        <v>36</v>
+      </c>
+      <c r="AH32">
+        <v>1</v>
+      </c>
+      <c r="AI32">
+        <v>1</v>
+      </c>
+      <c r="AJ32">
+        <v>0.3</v>
+      </c>
+      <c r="AK32">
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <v>0</v>
+      </c>
+      <c r="AM32">
+        <v>81</v>
+      </c>
+      <c r="AN32">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO32">
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33">
+        <v>0.21148581</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <v>0.86</v>
+      </c>
+      <c r="F33">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="G33">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>15</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <v>10</v>
+      </c>
+      <c r="N33">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="O33">
+        <v>81300.813008130077</v>
+      </c>
+      <c r="P33">
+        <v>0.71</v>
+      </c>
+      <c r="Q33">
+        <v>8</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>0.10529488625655987</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33">
+        <v>1</v>
+      </c>
+      <c r="Y33">
+        <v>1</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>1</v>
+      </c>
+      <c r="AB33">
+        <v>0.21135000000000001</v>
+      </c>
+      <c r="AC33">
+        <v>0.41692469000000004</v>
+      </c>
+      <c r="AD33">
+        <v>3.49735</v>
+      </c>
+      <c r="AE33">
+        <v>1.3430106357425033</v>
+      </c>
+      <c r="AF33">
+        <v>7</v>
+      </c>
+      <c r="AG33">
+        <v>40</v>
+      </c>
+      <c r="AH33">
+        <v>1</v>
+      </c>
+      <c r="AI33">
+        <v>1</v>
+      </c>
+      <c r="AJ33">
+        <v>0.35</v>
+      </c>
+      <c r="AK33">
+        <v>0.35</v>
+      </c>
+      <c r="AL33">
+        <v>0</v>
+      </c>
+      <c r="AM33">
+        <v>93</v>
+      </c>
+      <c r="AN33">
+        <v>0</v>
+      </c>
+      <c r="AO33">
+        <v>0</v>
+      </c>
+      <c r="AP33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34">
+        <v>0.22</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>0.876</v>
+      </c>
+      <c r="F34">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G34">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>45</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>9</v>
+      </c>
+      <c r="N34">
+        <v>0.18</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0.42</v>
+      </c>
+      <c r="Q34">
+        <v>91</v>
+      </c>
+      <c r="R34">
+        <v>0.5</v>
+      </c>
+      <c r="S34">
+        <v>0.31576253288366624</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>1</v>
+      </c>
+      <c r="Y34">
+        <v>1</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>1</v>
+      </c>
+      <c r="AB34">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AC34">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="AD34">
+        <v>3.2105969999999999</v>
+      </c>
+      <c r="AE34">
+        <v>1.2065660008024217</v>
+      </c>
+      <c r="AF34">
+        <v>1</v>
+      </c>
+      <c r="AG34">
+        <v>80</v>
+      </c>
+      <c r="AH34">
+        <v>1</v>
+      </c>
+      <c r="AI34">
+        <v>1</v>
+      </c>
+      <c r="AJ34">
+        <v>0.15</v>
+      </c>
+      <c r="AK34">
+        <v>0.1</v>
+      </c>
+      <c r="AL34">
+        <v>0.2</v>
+      </c>
+      <c r="AM34">
+        <v>84</v>
+      </c>
+      <c r="AN34">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO34">
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35">
+        <v>0.19</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>50</v>
+      </c>
+      <c r="E35">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>37</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>6</v>
+      </c>
+      <c r="N35">
+        <v>0.2</v>
+      </c>
+      <c r="O35">
+        <v>121428.57142857143</v>
+      </c>
+      <c r="P35">
+        <v>0.44</v>
+      </c>
+      <c r="Q35">
+        <v>25</v>
+      </c>
+      <c r="R35">
+        <v>0.5</v>
+      </c>
+      <c r="S35">
+        <v>2.531121421878852</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+      <c r="V35">
+        <v>1</v>
+      </c>
+      <c r="W35">
+        <v>1</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
+      <c r="Z35">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="AC35">
+        <v>0.47</v>
+      </c>
+      <c r="AD35">
+        <v>3.925891</v>
+      </c>
+      <c r="AE35">
+        <v>1.3961178782024719</v>
+      </c>
+      <c r="AF35">
+        <v>1</v>
+      </c>
+      <c r="AG35">
+        <v>48</v>
+      </c>
+      <c r="AH35">
+        <v>1</v>
+      </c>
+      <c r="AI35">
+        <v>1</v>
+      </c>
+      <c r="AJ35">
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <v>0.2</v>
+      </c>
+      <c r="AL35">
+        <v>0.2</v>
+      </c>
+      <c r="AM35">
+        <v>131</v>
+      </c>
+      <c r="AN35">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO35">
+        <v>0</v>
+      </c>
+      <c r="AP35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36">
+        <v>0.2583858</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>80</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0.35</v>
+      </c>
+      <c r="G36">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>87</v>
+      </c>
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <v>5</v>
+      </c>
+      <c r="N36">
+        <v>7.3648000000000005E-2</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0.4</v>
+      </c>
+      <c r="Q36">
+        <v>33</v>
+      </c>
+      <c r="R36">
+        <v>0.5</v>
+      </c>
+      <c r="S36">
+        <v>2.0923174000470826</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="V36">
+        <v>1</v>
+      </c>
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+      <c r="Y36">
+        <v>1</v>
+      </c>
+      <c r="Z36">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="AA36">
+        <v>0</v>
+      </c>
+      <c r="AB36">
+        <v>0.29240840000000001</v>
+      </c>
+      <c r="AC36">
+        <v>0.46</v>
+      </c>
+      <c r="AD36">
+        <v>9.4</v>
+      </c>
+      <c r="AE36">
+        <v>1.2514742986570191</v>
+      </c>
+      <c r="AF36">
+        <v>4</v>
+      </c>
+      <c r="AG36">
+        <v>55</v>
+      </c>
+      <c r="AH36">
+        <v>1</v>
+      </c>
+      <c r="AI36">
+        <v>0</v>
+      </c>
+      <c r="AJ36">
+        <v>0.3</v>
+      </c>
+      <c r="AK36">
+        <v>0.3</v>
+      </c>
+      <c r="AL36">
+        <v>0.3</v>
+      </c>
+      <c r="AM36">
+        <v>58</v>
+      </c>
+      <c r="AN36">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="AO36">
+        <v>0</v>
+      </c>
+      <c r="AP36">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -63725,7 +68334,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN23" sqref="AN23"/>
+      <selection pane="bottomRight" activeCell="T23" sqref="A1:AP36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>